<commit_message>
feat: add language info to text list
</commit_message>
<xml_diff>
--- a/docs/overview.xlsx
+++ b/docs/overview.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtwente/Desktop/modelling-marti/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtwente/github/modelling-marti/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6B683FF3-DAA0-7A42-A56C-77C3D396FA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCCAA227-36A1-7249-A8BB-2FA4FDB801C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CD469514-C64D-AA44-8D8D-7EECB4F4C723}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="articles" localSheetId="0">overview!$A$1:$B$189</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,7 +116,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{4BA58595-9323-474A-B01A-F661996FC8A7}" name="articles" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/mtwente/Desktop/modelling-marti/articles.csv" thousands="’" tab="0" comma="1">
+    <textPr sourceFile="/Users/mtwente/Desktop/modelling-marti/articles.csv" thousands="’" tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="389">
   <si>
     <t>NZZ_19520427_0025</t>
   </si>
@@ -1284,25 +1285,28 @@
   </si>
   <si>
     <t>Gedanken zur Beurteilung von Hochhausprojekten I</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1337,13 +1341,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1717,11 +1720,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2909730C-830C-7C42-AB69-BB3507A2110D}">
-  <dimension ref="A1:G189"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1733,7 @@
     <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>348</v>
       </c>
@@ -1744,16 +1747,19 @@
         <v>354</v>
       </c>
       <c r="E1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" t="s">
         <v>378</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>383</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1766,11 +1772,14 @@
       <c r="D2" s="2">
         <v>19091</v>
       </c>
-      <c r="E2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1783,11 +1792,14 @@
       <c r="D3" s="2">
         <v>19118</v>
       </c>
-      <c r="E3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1800,11 +1812,14 @@
       <c r="D4" s="2">
         <v>19132</v>
       </c>
-      <c r="E4" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1817,11 +1832,14 @@
       <c r="D5" s="2">
         <v>19146</v>
       </c>
-      <c r="E5" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1834,11 +1852,14 @@
       <c r="D6" s="2">
         <v>19171</v>
       </c>
-      <c r="E6" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1851,11 +1872,14 @@
       <c r="D7" s="2">
         <v>19186</v>
       </c>
-      <c r="E7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1868,11 +1892,14 @@
       <c r="D8" s="2">
         <v>19213</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F8" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1885,11 +1912,14 @@
       <c r="D9" s="2">
         <v>19214</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F9" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1902,11 +1932,14 @@
       <c r="D10" s="2">
         <v>19244</v>
       </c>
-      <c r="E10" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1919,11 +1952,14 @@
       <c r="D11" s="2">
         <v>19299</v>
       </c>
-      <c r="E11" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F11" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1936,11 +1972,14 @@
       <c r="D12" s="2">
         <v>19333</v>
       </c>
-      <c r="E12" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F12" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1953,11 +1992,14 @@
       <c r="D13" s="2">
         <v>19334</v>
       </c>
-      <c r="E13" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1970,11 +2012,14 @@
       <c r="D14" s="2">
         <v>19458</v>
       </c>
-      <c r="E14" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1987,11 +2032,14 @@
       <c r="D15" s="2">
         <v>19628</v>
       </c>
-      <c r="E15" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2004,11 +2052,14 @@
       <c r="D16" s="2">
         <v>20125</v>
       </c>
-      <c r="E16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2021,11 +2072,14 @@
       <c r="D17" s="2">
         <v>20663</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F17" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2038,11 +2092,14 @@
       <c r="D18" s="2">
         <v>20664</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F18" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2055,11 +2112,14 @@
       <c r="D19" s="2">
         <v>20770</v>
       </c>
-      <c r="E19" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F19" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2072,11 +2132,14 @@
       <c r="D20" s="2">
         <v>20783</v>
       </c>
-      <c r="E20" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2089,11 +2152,14 @@
       <c r="D21" s="2">
         <v>20842</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F21" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2106,11 +2172,14 @@
       <c r="D22" s="2">
         <v>20843</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F22" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2123,11 +2192,14 @@
       <c r="D23" s="2">
         <v>21216</v>
       </c>
-      <c r="E23" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F23" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2140,11 +2212,14 @@
       <c r="D24" s="2">
         <v>21682</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F24" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2157,11 +2232,14 @@
       <c r="D25" s="2">
         <v>21683</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F25" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2174,11 +2252,14 @@
       <c r="D26" s="2">
         <v>21684</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F26" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2191,11 +2272,14 @@
       <c r="D27" s="2">
         <v>21687</v>
       </c>
-      <c r="E27" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F27" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2208,11 +2292,14 @@
       <c r="D28" s="2">
         <v>22225</v>
       </c>
-      <c r="E28" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F28" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2225,11 +2312,14 @@
       <c r="D29" s="2">
         <v>22240</v>
       </c>
-      <c r="E29" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F29" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2242,11 +2332,14 @@
       <c r="D30" s="2">
         <v>22251</v>
       </c>
-      <c r="E30" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F30" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2259,11 +2352,14 @@
       <c r="D31" s="2">
         <v>22315</v>
       </c>
-      <c r="E31" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F31" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2276,11 +2372,14 @@
       <c r="D32" s="2">
         <v>22428</v>
       </c>
-      <c r="E32" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2293,11 +2392,14 @@
       <c r="D33" s="2">
         <v>22532</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F33" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2310,11 +2412,14 @@
       <c r="D34" s="2">
         <v>22532</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F34" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2327,11 +2432,14 @@
       <c r="D35" s="2">
         <v>22721</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F35" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2344,11 +2452,14 @@
       <c r="D36" s="2">
         <v>22721</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F36" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2361,11 +2472,14 @@
       <c r="D37" s="2">
         <v>22725</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F37" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2378,11 +2492,14 @@
       <c r="D38" s="2">
         <v>22734</v>
       </c>
-      <c r="E38" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F38" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2395,11 +2512,14 @@
       <c r="D39" s="2">
         <v>23086</v>
       </c>
-      <c r="E39" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F39" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2412,11 +2532,14 @@
       <c r="D40" s="2">
         <v>23178</v>
       </c>
-      <c r="E40" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F40" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2429,11 +2552,14 @@
       <c r="D41" s="2">
         <v>23972</v>
       </c>
-      <c r="E41" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F41" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2446,11 +2572,14 @@
       <c r="D42" s="2">
         <v>24155</v>
       </c>
-      <c r="E42" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F42" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -2463,11 +2592,14 @@
       <c r="D43" s="2">
         <v>24181</v>
       </c>
-      <c r="E43" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F43" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2480,11 +2612,14 @@
       <c r="D44" s="2">
         <v>24252</v>
       </c>
-      <c r="E44" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F44" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2497,11 +2632,14 @@
       <c r="D45" s="2">
         <v>24446</v>
       </c>
-      <c r="E45" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E45" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F45" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -2514,11 +2652,14 @@
       <c r="D46" s="2">
         <v>24928</v>
       </c>
-      <c r="E46" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E46" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F46" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -2531,11 +2672,14 @@
       <c r="D47" s="2">
         <v>25142</v>
       </c>
-      <c r="E47" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F47" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2548,11 +2692,14 @@
       <c r="D48" s="2">
         <v>25573</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F48" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -2565,11 +2712,14 @@
       <c r="D49" s="2">
         <v>25574</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F49" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -2582,11 +2732,14 @@
       <c r="D50" s="2">
         <v>25575</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F50" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2599,11 +2752,14 @@
       <c r="D51" s="2">
         <v>25637</v>
       </c>
-      <c r="E51" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E51" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F51" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2616,11 +2772,14 @@
       <c r="D52" s="2">
         <v>25651</v>
       </c>
-      <c r="E52" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E52" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F52" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2633,11 +2792,14 @@
       <c r="D53" s="2">
         <v>27152</v>
       </c>
-      <c r="E53" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E53" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F53" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2650,11 +2812,14 @@
       <c r="D54" s="2">
         <v>27499</v>
       </c>
-      <c r="E54" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E54" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F54" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2667,11 +2832,14 @@
       <c r="D55" s="2">
         <v>27628</v>
       </c>
-      <c r="E55" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E55" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F55" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2684,11 +2852,14 @@
       <c r="D56" s="2">
         <v>30772</v>
       </c>
-      <c r="E56" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E56" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F56" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2701,11 +2872,14 @@
       <c r="D57" s="2">
         <v>31090</v>
       </c>
-      <c r="E57" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E57" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F57" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2718,11 +2892,14 @@
       <c r="D58" s="2">
         <v>32626</v>
       </c>
-      <c r="E58" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E58" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F58" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2735,17 +2912,20 @@
       <c r="D59" s="3">
         <v>1951</v>
       </c>
-      <c r="E59" t="s">
-        <v>382</v>
-      </c>
-      <c r="F59">
+      <c r="E59" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F59" t="s">
+        <v>382</v>
+      </c>
+      <c r="G59">
         <v>9</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2758,17 +2938,20 @@
       <c r="D60" s="2">
         <v>22616</v>
       </c>
-      <c r="E60" t="s">
-        <v>382</v>
-      </c>
-      <c r="F60">
+      <c r="E60" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F60" t="s">
+        <v>382</v>
+      </c>
+      <c r="G60">
         <v>9</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2781,17 +2964,20 @@
       <c r="D61" s="3">
         <v>1960</v>
       </c>
-      <c r="E61" t="s">
-        <v>382</v>
-      </c>
-      <c r="F61">
+      <c r="E61" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F61" t="s">
+        <v>382</v>
+      </c>
+      <c r="G61">
         <v>8</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2804,17 +2990,20 @@
       <c r="D62" s="2">
         <v>22525</v>
       </c>
-      <c r="E62" t="s">
-        <v>382</v>
-      </c>
-      <c r="F62">
+      <c r="E62" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F62" t="s">
+        <v>382</v>
+      </c>
+      <c r="G62">
         <v>10</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>693</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2827,17 +3016,20 @@
       <c r="D63" s="2">
         <v>23651</v>
       </c>
-      <c r="E63" t="s">
-        <v>382</v>
-      </c>
-      <c r="F63">
+      <c r="E63" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F63" t="s">
+        <v>382</v>
+      </c>
+      <c r="G63">
         <v>12</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2850,17 +3042,20 @@
       <c r="D64" s="2">
         <v>23377</v>
       </c>
-      <c r="E64" t="s">
-        <v>382</v>
-      </c>
-      <c r="F64">
+      <c r="E64" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F64" t="s">
+        <v>382</v>
+      </c>
+      <c r="G64">
         <v>12</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>311</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2873,17 +3068,20 @@
       <c r="D65" s="3">
         <v>1946</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F65" t="s">
         <v>379</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>11</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>728</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2896,17 +3094,20 @@
       <c r="D66" s="3">
         <v>1946</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F66" t="s">
         <v>379</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>11</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>331</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2919,17 +3120,20 @@
       <c r="D67" s="3">
         <v>1946</v>
       </c>
-      <c r="E67" t="s">
-        <v>382</v>
-      </c>
-      <c r="F67">
+      <c r="E67" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F67" t="s">
+        <v>382</v>
+      </c>
+      <c r="G67">
         <v>24</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>271</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -2942,17 +3146,20 @@
       <c r="D68" s="3">
         <v>1947</v>
       </c>
-      <c r="E68" t="s">
-        <v>382</v>
-      </c>
-      <c r="F68">
+      <c r="E68" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F68" t="s">
+        <v>382</v>
+      </c>
+      <c r="G68">
         <v>27</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>944</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2965,17 +3172,20 @@
       <c r="D69" s="3">
         <v>1948</v>
       </c>
-      <c r="E69" t="s">
-        <v>382</v>
-      </c>
-      <c r="F69">
+      <c r="E69" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F69" t="s">
+        <v>382</v>
+      </c>
+      <c r="G69">
         <v>15</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2988,17 +3198,20 @@
       <c r="D70" s="3">
         <v>1949</v>
       </c>
-      <c r="E70" t="s">
-        <v>382</v>
-      </c>
-      <c r="F70">
+      <c r="E70" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F70" t="s">
+        <v>382</v>
+      </c>
+      <c r="G70">
         <v>21</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>2582</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -3011,17 +3224,20 @@
       <c r="D71" s="2">
         <v>18445</v>
       </c>
-      <c r="E71" t="s">
-        <v>382</v>
-      </c>
-      <c r="F71">
+      <c r="E71" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F71" t="s">
+        <v>382</v>
+      </c>
+      <c r="G71">
         <v>9</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>1171</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -3034,17 +3250,20 @@
       <c r="D72" s="3">
         <v>1950</v>
       </c>
-      <c r="E72" t="s">
-        <v>382</v>
-      </c>
-      <c r="F72">
+      <c r="E72" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F72" t="s">
+        <v>382</v>
+      </c>
+      <c r="G72">
         <v>20</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>333</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -3057,17 +3276,20 @@
       <c r="D73" s="3">
         <v>1951</v>
       </c>
-      <c r="E73" t="s">
-        <v>382</v>
-      </c>
-      <c r="F73">
+      <c r="E73" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F73" t="s">
+        <v>382</v>
+      </c>
+      <c r="G73">
         <v>13</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>379</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -3080,17 +3302,20 @@
       <c r="D74" s="2">
         <v>19238</v>
       </c>
-      <c r="E74" t="s">
-        <v>382</v>
-      </c>
-      <c r="F74">
+      <c r="E74" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F74" t="s">
+        <v>382</v>
+      </c>
+      <c r="G74">
         <v>16</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>863</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -3103,17 +3328,20 @@
       <c r="D75" s="2">
         <v>19541</v>
       </c>
-      <c r="E75" t="s">
-        <v>382</v>
-      </c>
-      <c r="F75">
+      <c r="E75" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F75" t="s">
+        <v>382</v>
+      </c>
+      <c r="G75">
         <v>10</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>718</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -3126,17 +3354,20 @@
       <c r="D76" s="2">
         <v>20394</v>
       </c>
-      <c r="E76" t="s">
-        <v>382</v>
-      </c>
-      <c r="F76">
+      <c r="E76" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F76" t="s">
+        <v>382</v>
+      </c>
+      <c r="G76">
         <v>10</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>337</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -3149,17 +3380,20 @@
       <c r="D77" s="3">
         <v>1963</v>
       </c>
-      <c r="E77" t="s">
-        <v>382</v>
-      </c>
-      <c r="F77">
+      <c r="E77" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F77" t="s">
+        <v>382</v>
+      </c>
+      <c r="G77">
         <v>63</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3172,17 +3406,20 @@
       <c r="D78" s="3">
         <v>1963</v>
       </c>
-      <c r="E78" t="s">
-        <v>382</v>
-      </c>
-      <c r="F78">
+      <c r="E78" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F78" t="s">
+        <v>382</v>
+      </c>
+      <c r="G78">
         <v>23</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>365</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -3195,17 +3432,20 @@
       <c r="D79" s="3">
         <v>1964</v>
       </c>
-      <c r="E79" t="s">
-        <v>382</v>
-      </c>
-      <c r="F79">
+      <c r="E79" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F79" t="s">
+        <v>382</v>
+      </c>
+      <c r="G79">
         <v>22</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>997</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -3218,17 +3458,20 @@
       <c r="D80" s="3">
         <v>1968</v>
       </c>
-      <c r="E80" t="s">
-        <v>382</v>
-      </c>
-      <c r="F80">
+      <c r="E80" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F80" t="s">
+        <v>382</v>
+      </c>
+      <c r="G80">
         <v>9</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -3241,17 +3484,20 @@
       <c r="D81" s="3">
         <v>1969</v>
       </c>
-      <c r="E81" t="s">
-        <v>382</v>
-      </c>
-      <c r="F81">
+      <c r="E81" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F81" t="s">
+        <v>382</v>
+      </c>
+      <c r="G81">
         <v>11</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>330</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -3264,17 +3510,20 @@
       <c r="D82" s="2">
         <v>26085</v>
       </c>
-      <c r="E82" t="s">
-        <v>382</v>
-      </c>
-      <c r="F82">
+      <c r="E82" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F82" t="s">
+        <v>382</v>
+      </c>
+      <c r="G82">
         <v>9</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>608</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -3287,17 +3536,20 @@
       <c r="D83" s="2">
         <v>18025</v>
       </c>
-      <c r="E83" t="s">
-        <v>382</v>
-      </c>
-      <c r="F83">
+      <c r="E83" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F83" t="s">
+        <v>382</v>
+      </c>
+      <c r="G83">
         <v>33</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3310,17 +3562,20 @@
       <c r="D84" s="2">
         <v>18053</v>
       </c>
-      <c r="E84" t="s">
-        <v>382</v>
-      </c>
-      <c r="F84">
+      <c r="E84" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F84" t="s">
+        <v>382</v>
+      </c>
+      <c r="G84">
         <v>144</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>523</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -3333,17 +3588,20 @@
       <c r="D85" s="2">
         <v>18060</v>
       </c>
-      <c r="E85" t="s">
-        <v>382</v>
-      </c>
-      <c r="F85">
+      <c r="E85" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F85" t="s">
+        <v>382</v>
+      </c>
+      <c r="G85">
         <v>101</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>303</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -3356,17 +3614,20 @@
       <c r="D86" s="2">
         <v>18130</v>
       </c>
-      <c r="E86" t="s">
-        <v>382</v>
-      </c>
-      <c r="F86">
+      <c r="E86" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F86" t="s">
+        <v>382</v>
+      </c>
+      <c r="G86">
         <v>15</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>635</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -3379,17 +3640,20 @@
       <c r="D87" s="2">
         <v>18151</v>
       </c>
-      <c r="E87" t="s">
-        <v>382</v>
-      </c>
-      <c r="F87">
+      <c r="E87" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F87" t="s">
+        <v>382</v>
+      </c>
+      <c r="G87">
         <v>26</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>859</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -3402,17 +3666,20 @@
       <c r="D88" s="2">
         <v>18186</v>
       </c>
-      <c r="E88" t="s">
-        <v>382</v>
-      </c>
-      <c r="F88">
+      <c r="E88" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F88" t="s">
+        <v>382</v>
+      </c>
+      <c r="G88">
         <v>93</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>658</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3425,17 +3692,20 @@
       <c r="D89" s="2">
         <v>18242</v>
       </c>
-      <c r="E89" t="s">
-        <v>382</v>
-      </c>
-      <c r="F89">
+      <c r="E89" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F89" t="s">
+        <v>382</v>
+      </c>
+      <c r="G89">
         <v>126</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>417</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -3448,17 +3718,20 @@
       <c r="D90" s="2">
         <v>18256</v>
       </c>
-      <c r="E90" t="s">
-        <v>382</v>
-      </c>
-      <c r="F90">
+      <c r="E90" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F90" t="s">
+        <v>382</v>
+      </c>
+      <c r="G90">
         <v>161</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>217</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -3471,17 +3744,20 @@
       <c r="D91" s="2">
         <v>18424</v>
       </c>
-      <c r="E91" t="s">
-        <v>382</v>
-      </c>
-      <c r="F91">
+      <c r="E91" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F91" t="s">
+        <v>382</v>
+      </c>
+      <c r="G91">
         <v>41</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -3494,17 +3770,20 @@
       <c r="D92" s="2">
         <v>18522</v>
       </c>
-      <c r="E92" t="s">
-        <v>382</v>
-      </c>
-      <c r="F92">
+      <c r="E92" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F92" t="s">
+        <v>382</v>
+      </c>
+      <c r="G92">
         <v>110</v>
       </c>
-      <c r="G92">
+      <c r="H92">
         <v>987</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -3517,17 +3796,20 @@
       <c r="D93" s="2">
         <v>18844</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F93" t="s">
         <v>379</v>
       </c>
-      <c r="F93">
+      <c r="G93">
         <v>15</v>
       </c>
-      <c r="G93">
+      <c r="H93">
         <v>795</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -3540,17 +3822,20 @@
       <c r="D94" s="2">
         <v>18851</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F94" t="s">
         <v>379</v>
       </c>
-      <c r="F94">
+      <c r="G94">
         <v>17</v>
       </c>
-      <c r="G94">
+      <c r="H94">
         <v>642</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -3563,17 +3848,20 @@
       <c r="D95" s="2">
         <v>18928</v>
       </c>
-      <c r="E95" t="s">
-        <v>382</v>
-      </c>
-      <c r="F95">
+      <c r="E95" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F95" t="s">
+        <v>382</v>
+      </c>
+      <c r="G95">
         <v>26</v>
       </c>
-      <c r="G95">
+      <c r="H95">
         <v>597</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3586,17 +3874,20 @@
       <c r="D96" s="2">
         <v>18977</v>
       </c>
-      <c r="E96" t="s">
-        <v>382</v>
-      </c>
-      <c r="F96">
+      <c r="E96" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F96" t="s">
+        <v>382</v>
+      </c>
+      <c r="G96">
         <v>120</v>
       </c>
-      <c r="G96">
+      <c r="H96">
         <v>891</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -3609,17 +3900,20 @@
       <c r="D97" s="2">
         <v>19103</v>
       </c>
-      <c r="E97" t="s">
-        <v>382</v>
-      </c>
-      <c r="F97">
+      <c r="E97" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F97" t="s">
+        <v>382</v>
+      </c>
+      <c r="G97">
         <v>66</v>
       </c>
-      <c r="G97">
+      <c r="H97">
         <v>345</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -3632,17 +3926,20 @@
       <c r="D98" s="2">
         <v>19194</v>
       </c>
-      <c r="E98" t="s">
-        <v>382</v>
-      </c>
-      <c r="F98">
+      <c r="E98" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F98" t="s">
+        <v>382</v>
+      </c>
+      <c r="G98">
         <v>14</v>
       </c>
-      <c r="G98">
+      <c r="H98">
         <v>286</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -3655,17 +3952,20 @@
       <c r="D99" s="2">
         <v>19208</v>
       </c>
-      <c r="E99" t="s">
-        <v>382</v>
-      </c>
-      <c r="F99">
+      <c r="E99" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F99" t="s">
+        <v>382</v>
+      </c>
+      <c r="G99">
         <v>133</v>
       </c>
-      <c r="G99">
+      <c r="H99">
         <v>532</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -3678,17 +3978,20 @@
       <c r="D100" s="2">
         <v>19215</v>
       </c>
-      <c r="E100" t="s">
-        <v>382</v>
-      </c>
-      <c r="F100">
+      <c r="E100" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F100" t="s">
+        <v>382</v>
+      </c>
+      <c r="G100">
         <v>32</v>
       </c>
-      <c r="G100">
+      <c r="H100">
         <v>601</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -3701,17 +4004,20 @@
       <c r="D101" s="2">
         <v>19327</v>
       </c>
-      <c r="E101" t="s">
-        <v>382</v>
-      </c>
-      <c r="F101">
+      <c r="E101" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F101" t="s">
+        <v>382</v>
+      </c>
+      <c r="G101">
         <v>223</v>
       </c>
-      <c r="G101">
+      <c r="H101">
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -3724,17 +4030,20 @@
       <c r="D102" s="2">
         <v>19369</v>
       </c>
-      <c r="E102" t="s">
-        <v>382</v>
-      </c>
-      <c r="F102">
+      <c r="E102" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F102" t="s">
+        <v>382</v>
+      </c>
+      <c r="G102">
         <v>26</v>
       </c>
-      <c r="G102">
+      <c r="H102">
         <v>208</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -3747,17 +4056,20 @@
       <c r="D103" s="2">
         <v>19509</v>
       </c>
-      <c r="E103" t="s">
-        <v>382</v>
-      </c>
-      <c r="F103">
+      <c r="E103" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F103" t="s">
+        <v>382</v>
+      </c>
+      <c r="G103">
         <v>102</v>
       </c>
-      <c r="G103">
+      <c r="H103">
         <v>890</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -3770,17 +4082,20 @@
       <c r="D104" s="2">
         <v>19537</v>
       </c>
-      <c r="E104" t="s">
-        <v>382</v>
-      </c>
-      <c r="F104">
+      <c r="E104" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F104" t="s">
+        <v>382</v>
+      </c>
+      <c r="G104">
         <v>100</v>
       </c>
-      <c r="G104">
+      <c r="H104">
         <v>594</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -3793,17 +4108,20 @@
       <c r="D105" s="2">
         <v>19544</v>
       </c>
-      <c r="E105" t="s">
-        <v>382</v>
-      </c>
-      <c r="F105">
+      <c r="E105" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F105" t="s">
+        <v>382</v>
+      </c>
+      <c r="G105">
         <v>14</v>
       </c>
-      <c r="G105">
+      <c r="H105">
         <v>592</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -3816,17 +4134,20 @@
       <c r="D106" s="2">
         <v>19614</v>
       </c>
-      <c r="E106" t="s">
-        <v>382</v>
-      </c>
-      <c r="F106">
+      <c r="E106" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F106" t="s">
+        <v>382</v>
+      </c>
+      <c r="G106">
         <v>39</v>
       </c>
-      <c r="G106">
+      <c r="H106">
         <v>91</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -3839,17 +4160,20 @@
       <c r="D107" s="2">
         <v>19635</v>
       </c>
-      <c r="E107" t="s">
-        <v>382</v>
-      </c>
-      <c r="F107">
+      <c r="E107" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F107" t="s">
+        <v>382</v>
+      </c>
+      <c r="G107">
         <v>19</v>
       </c>
-      <c r="G107">
+      <c r="H107">
         <v>192</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -3862,17 +4186,20 @@
       <c r="D108" s="2">
         <v>19670</v>
       </c>
-      <c r="E108" t="s">
-        <v>382</v>
-      </c>
-      <c r="F108">
+      <c r="E108" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F108" t="s">
+        <v>382</v>
+      </c>
+      <c r="G108">
         <v>72</v>
       </c>
-      <c r="G108">
+      <c r="H108">
         <v>393</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -3885,17 +4212,20 @@
       <c r="D109" s="2">
         <v>19670</v>
       </c>
-      <c r="E109" t="s">
-        <v>382</v>
-      </c>
-      <c r="F109">
+      <c r="E109" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F109" t="s">
+        <v>382</v>
+      </c>
+      <c r="G109">
         <v>68</v>
       </c>
-      <c r="G109">
+      <c r="H109">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -3908,17 +4238,20 @@
       <c r="D110" s="2">
         <v>19684</v>
       </c>
-      <c r="E110" t="s">
-        <v>382</v>
-      </c>
-      <c r="F110">
+      <c r="E110" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F110" t="s">
+        <v>382</v>
+      </c>
+      <c r="G110">
         <v>13</v>
       </c>
-      <c r="G110">
+      <c r="H110">
         <v>490</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -3931,17 +4264,20 @@
       <c r="D111" s="2">
         <v>19698</v>
       </c>
-      <c r="E111" t="s">
-        <v>382</v>
-      </c>
-      <c r="F111">
+      <c r="E111" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F111" t="s">
+        <v>382</v>
+      </c>
+      <c r="G111">
         <v>115</v>
       </c>
-      <c r="G111">
+      <c r="H111">
         <v>192</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -3954,17 +4290,20 @@
       <c r="D112" s="2">
         <v>19397</v>
       </c>
-      <c r="E112" t="s">
-        <v>382</v>
-      </c>
-      <c r="F112">
+      <c r="E112" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F112" t="s">
+        <v>382</v>
+      </c>
+      <c r="G112">
         <v>17</v>
       </c>
-      <c r="G112">
+      <c r="H112">
         <v>236</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -3977,17 +4316,20 @@
       <c r="D113" s="2">
         <v>19908</v>
       </c>
-      <c r="E113" t="s">
-        <v>382</v>
-      </c>
-      <c r="F113">
+      <c r="E113" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F113" t="s">
+        <v>382</v>
+      </c>
+      <c r="G113">
         <v>44</v>
       </c>
-      <c r="G113">
+      <c r="H113">
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -4000,17 +4342,20 @@
       <c r="D114" s="2">
         <v>19992</v>
       </c>
-      <c r="E114" t="s">
-        <v>382</v>
-      </c>
-      <c r="F114">
+      <c r="E114" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F114" t="s">
+        <v>382</v>
+      </c>
+      <c r="G114">
         <v>670</v>
       </c>
-      <c r="G114">
+      <c r="H114">
         <v>755</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -4023,17 +4368,20 @@
       <c r="D115" s="2">
         <v>19992</v>
       </c>
-      <c r="E115" t="s">
-        <v>382</v>
-      </c>
-      <c r="F115">
+      <c r="E115" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F115" t="s">
+        <v>382</v>
+      </c>
+      <c r="G115">
         <v>64</v>
       </c>
-      <c r="G115">
+      <c r="H115">
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -4046,17 +4394,20 @@
       <c r="D116" s="2">
         <v>20076</v>
       </c>
-      <c r="E116" t="s">
-        <v>382</v>
-      </c>
-      <c r="F116">
+      <c r="E116" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F116" t="s">
+        <v>382</v>
+      </c>
+      <c r="G116">
         <v>37</v>
       </c>
-      <c r="G116">
+      <c r="H116">
         <v>766</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -4069,17 +4420,20 @@
       <c r="D117" s="2">
         <v>20146</v>
       </c>
-      <c r="E117" t="s">
-        <v>382</v>
-      </c>
-      <c r="F117" s="4">
+      <c r="E117" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F117" t="s">
+        <v>382</v>
+      </c>
+      <c r="G117">
         <v>72</v>
       </c>
-      <c r="G117" s="4">
+      <c r="H117">
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -4092,17 +4446,20 @@
       <c r="D118" s="2">
         <v>20181</v>
       </c>
-      <c r="E118" t="s">
-        <v>382</v>
-      </c>
-      <c r="F118">
+      <c r="E118" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F118" t="s">
+        <v>382</v>
+      </c>
+      <c r="G118">
         <v>102</v>
       </c>
-      <c r="G118">
+      <c r="H118">
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -4115,17 +4472,20 @@
       <c r="D119" s="2">
         <v>20244</v>
       </c>
-      <c r="E119" t="s">
-        <v>382</v>
-      </c>
-      <c r="F119">
+      <c r="E119" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F119" t="s">
+        <v>382</v>
+      </c>
+      <c r="G119">
         <v>12</v>
       </c>
-      <c r="G119">
+      <c r="H119">
         <v>409</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -4138,17 +4498,20 @@
       <c r="D120" s="2">
         <v>20258</v>
       </c>
-      <c r="E120" t="s">
-        <v>382</v>
-      </c>
-      <c r="F120">
+      <c r="E120" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F120" t="s">
+        <v>382</v>
+      </c>
+      <c r="G120">
         <v>23</v>
       </c>
-      <c r="G120">
+      <c r="H120">
         <v>179</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -4161,17 +4524,20 @@
       <c r="D121" s="2">
         <v>20111</v>
       </c>
-      <c r="E121" t="s">
-        <v>382</v>
-      </c>
-      <c r="F121">
+      <c r="E121" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F121" t="s">
+        <v>382</v>
+      </c>
+      <c r="G121">
         <v>77</v>
       </c>
-      <c r="G121">
+      <c r="H121">
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -4184,17 +4550,20 @@
       <c r="D122" s="2">
         <v>20370</v>
       </c>
-      <c r="E122" t="s">
-        <v>382</v>
-      </c>
-      <c r="F122">
+      <c r="E122" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F122" t="s">
+        <v>382</v>
+      </c>
+      <c r="G122">
         <v>75</v>
       </c>
-      <c r="G122">
+      <c r="H122">
         <v>550</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -4207,17 +4576,20 @@
       <c r="D123" s="2">
         <v>20412</v>
       </c>
-      <c r="E123" t="s">
-        <v>382</v>
-      </c>
-      <c r="F123">
+      <c r="E123" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F123" t="s">
+        <v>382</v>
+      </c>
+      <c r="G123">
         <v>80</v>
       </c>
-      <c r="G123">
+      <c r="H123">
         <v>169</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -4230,17 +4602,20 @@
       <c r="D124" s="2">
         <v>20545</v>
       </c>
-      <c r="E124" t="s">
-        <v>382</v>
-      </c>
-      <c r="F124">
+      <c r="E124" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F124" t="s">
+        <v>382</v>
+      </c>
+      <c r="G124">
         <v>11</v>
       </c>
-      <c r="G124">
+      <c r="H124">
         <v>202</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -4253,17 +4628,20 @@
       <c r="D125" s="2">
         <v>20601</v>
       </c>
-      <c r="E125" t="s">
-        <v>382</v>
-      </c>
-      <c r="F125">
+      <c r="E125" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F125" t="s">
+        <v>382</v>
+      </c>
+      <c r="G125">
         <v>146</v>
       </c>
-      <c r="G125">
+      <c r="H125">
         <v>300</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -4276,17 +4654,20 @@
       <c r="D126" s="2">
         <v>20636</v>
       </c>
-      <c r="E126" t="s">
-        <v>382</v>
-      </c>
-      <c r="F126">
+      <c r="E126" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F126" t="s">
+        <v>382</v>
+      </c>
+      <c r="G126">
         <v>46</v>
       </c>
-      <c r="G126">
+      <c r="H126">
         <v>292</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -4299,17 +4680,20 @@
       <c r="D127" s="2">
         <v>20636</v>
       </c>
-      <c r="E127" t="s">
-        <v>382</v>
-      </c>
-      <c r="F127">
+      <c r="E127" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F127" t="s">
+        <v>382</v>
+      </c>
+      <c r="G127">
         <v>57</v>
       </c>
-      <c r="G127">
+      <c r="H127">
         <v>81</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -4322,17 +4706,20 @@
       <c r="D128" s="2">
         <v>20748</v>
       </c>
-      <c r="E128" t="s">
-        <v>382</v>
-      </c>
-      <c r="F128">
+      <c r="E128" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F128" t="s">
+        <v>382</v>
+      </c>
+      <c r="G128">
         <v>11</v>
       </c>
-      <c r="G128">
+      <c r="H128">
         <v>53</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -4345,17 +4732,20 @@
       <c r="D129" s="2">
         <v>20769</v>
       </c>
-      <c r="E129" t="s">
-        <v>382</v>
-      </c>
-      <c r="F129">
+      <c r="E129" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F129" t="s">
+        <v>382</v>
+      </c>
+      <c r="G129">
         <v>11</v>
       </c>
-      <c r="G129">
+      <c r="H129">
         <v>879</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -4368,17 +4758,20 @@
       <c r="D130" s="2">
         <v>20783</v>
       </c>
-      <c r="E130" t="s">
-        <v>382</v>
-      </c>
-      <c r="F130">
+      <c r="E130" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F130" t="s">
+        <v>382</v>
+      </c>
+      <c r="G130">
         <v>28</v>
       </c>
-      <c r="G130">
+      <c r="H130">
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -4391,17 +4784,20 @@
       <c r="D131" s="2">
         <v>20790</v>
       </c>
-      <c r="E131" t="s">
-        <v>382</v>
-      </c>
-      <c r="F131">
+      <c r="E131" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F131" t="s">
+        <v>382</v>
+      </c>
+      <c r="G131">
         <v>62</v>
       </c>
-      <c r="G131">
+      <c r="H131">
         <v>209</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -4414,17 +4810,20 @@
       <c r="D132" s="2">
         <v>20888</v>
       </c>
-      <c r="E132" t="s">
-        <v>382</v>
-      </c>
-      <c r="F132">
+      <c r="E132" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F132" t="s">
+        <v>382</v>
+      </c>
+      <c r="G132">
         <v>29</v>
       </c>
-      <c r="G132">
+      <c r="H132">
         <v>461</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -4437,17 +4836,20 @@
       <c r="D133" s="2">
         <v>20902</v>
       </c>
-      <c r="E133" t="s">
-        <v>382</v>
-      </c>
-      <c r="F133">
+      <c r="E133" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F133" t="s">
+        <v>382</v>
+      </c>
+      <c r="G133">
         <v>14</v>
       </c>
-      <c r="G133">
+      <c r="H133">
         <v>519</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -4460,17 +4862,20 @@
       <c r="D134" s="2">
         <v>21035</v>
       </c>
-      <c r="E134" t="s">
-        <v>382</v>
-      </c>
-      <c r="F134">
+      <c r="E134" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F134" t="s">
+        <v>382</v>
+      </c>
+      <c r="G134">
         <v>81</v>
       </c>
-      <c r="G134">
+      <c r="H134">
         <v>269</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -4483,17 +4888,20 @@
       <c r="D135" s="2">
         <v>21126</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F135" t="s">
         <v>379</v>
       </c>
-      <c r="F135">
+      <c r="G135">
         <v>60</v>
       </c>
-      <c r="G135">
+      <c r="H135">
         <v>378</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -4506,17 +4914,20 @@
       <c r="D136" s="2">
         <v>21133</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F136" t="s">
         <v>379</v>
       </c>
-      <c r="F136">
+      <c r="G136">
         <v>69</v>
       </c>
-      <c r="G136">
+      <c r="H136">
         <v>369</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -4529,17 +4940,20 @@
       <c r="D137" s="2">
         <v>21140</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F137" t="s">
         <v>379</v>
       </c>
-      <c r="F137">
+      <c r="G137">
         <v>14</v>
       </c>
-      <c r="G137">
+      <c r="H137">
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -4552,17 +4966,20 @@
       <c r="D138" s="2">
         <v>21182</v>
       </c>
-      <c r="E138" t="s">
-        <v>382</v>
-      </c>
-      <c r="F138">
+      <c r="E138" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F138" t="s">
+        <v>382</v>
+      </c>
+      <c r="G138">
         <v>11</v>
       </c>
-      <c r="G138">
+      <c r="H138">
         <v>268</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -4575,17 +4992,20 @@
       <c r="D139" s="2">
         <v>21469</v>
       </c>
-      <c r="E139" t="s">
-        <v>382</v>
-      </c>
-      <c r="F139">
+      <c r="E139" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F139" t="s">
+        <v>382</v>
+      </c>
+      <c r="G139">
         <v>18</v>
       </c>
-      <c r="G139">
+      <c r="H139">
         <v>79</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -4598,17 +5018,20 @@
       <c r="D140" s="2">
         <v>21600</v>
       </c>
-      <c r="E140" t="s">
-        <v>382</v>
-      </c>
-      <c r="F140">
+      <c r="E140" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F140" t="s">
+        <v>382</v>
+      </c>
+      <c r="G140">
         <v>9</v>
       </c>
-      <c r="G140">
+      <c r="H140">
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -4621,17 +5044,20 @@
       <c r="D141" s="2">
         <v>21642</v>
       </c>
-      <c r="E141" t="s">
-        <v>382</v>
-      </c>
-      <c r="F141">
+      <c r="E141" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F141" t="s">
+        <v>382</v>
+      </c>
+      <c r="G141">
         <v>85</v>
       </c>
-      <c r="G141">
+      <c r="H141">
         <v>330</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -4644,17 +5070,20 @@
       <c r="D142" s="2">
         <v>21761</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F142" t="s">
         <v>379</v>
       </c>
-      <c r="F142">
+      <c r="G142">
         <v>83</v>
       </c>
-      <c r="G142">
+      <c r="H142">
         <v>485</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -4667,17 +5096,20 @@
       <c r="D143" s="2">
         <v>21768</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F143" t="s">
         <v>379</v>
       </c>
-      <c r="F143">
+      <c r="G143">
         <v>49</v>
       </c>
-      <c r="G143">
+      <c r="H143">
         <v>93</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>150</v>
       </c>
@@ -4690,17 +5122,20 @@
       <c r="D144" s="2">
         <v>21572</v>
       </c>
-      <c r="E144" t="s">
-        <v>382</v>
-      </c>
-      <c r="F144">
+      <c r="E144" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F144" t="s">
+        <v>382</v>
+      </c>
+      <c r="G144">
         <v>83</v>
       </c>
-      <c r="G144">
+      <c r="H144">
         <v>591</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -4713,17 +5148,20 @@
       <c r="D145" s="2">
         <v>21971</v>
       </c>
-      <c r="E145" t="s">
-        <v>382</v>
-      </c>
-      <c r="F145">
+      <c r="E145" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F145" t="s">
+        <v>382</v>
+      </c>
+      <c r="G145">
         <v>143</v>
       </c>
-      <c r="G145">
+      <c r="H145">
         <v>566</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>152</v>
       </c>
@@ -4736,17 +5174,20 @@
       <c r="D146" s="2">
         <v>22041</v>
       </c>
-      <c r="E146" t="s">
-        <v>382</v>
-      </c>
-      <c r="F146">
+      <c r="E146" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F146" t="s">
+        <v>382</v>
+      </c>
+      <c r="G146">
         <v>1003</v>
       </c>
-      <c r="G146">
+      <c r="H146">
         <v>1027</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -4759,17 +5200,20 @@
       <c r="D147" s="2">
         <v>22055</v>
       </c>
-      <c r="E147" t="s">
-        <v>382</v>
-      </c>
-      <c r="F147">
+      <c r="E147" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F147" t="s">
+        <v>382</v>
+      </c>
+      <c r="G147">
         <v>11</v>
       </c>
-      <c r="G147">
+      <c r="H147">
         <v>590</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -4782,17 +5226,20 @@
       <c r="D148" s="2">
         <v>22125</v>
       </c>
-      <c r="E148" t="s">
-        <v>382</v>
-      </c>
-      <c r="F148">
+      <c r="E148" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F148" t="s">
+        <v>382</v>
+      </c>
+      <c r="G148">
         <v>107</v>
       </c>
-      <c r="G148">
+      <c r="H148">
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -4805,17 +5252,20 @@
       <c r="D149" s="2">
         <v>22216</v>
       </c>
-      <c r="E149" t="s">
-        <v>382</v>
-      </c>
-      <c r="F149">
+      <c r="E149" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F149" t="s">
+        <v>382</v>
+      </c>
+      <c r="G149">
         <v>811</v>
       </c>
-      <c r="G149">
+      <c r="H149">
         <v>851</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>156</v>
       </c>
@@ -4828,17 +5278,20 @@
       <c r="D150" s="2">
         <v>22335</v>
       </c>
-      <c r="E150" t="s">
-        <v>382</v>
-      </c>
-      <c r="F150">
+      <c r="E150" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F150" t="s">
+        <v>382</v>
+      </c>
+      <c r="G150">
         <v>11</v>
       </c>
-      <c r="G150">
+      <c r="H150">
         <v>284</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -4851,17 +5304,20 @@
       <c r="D151" s="2">
         <v>22356</v>
       </c>
-      <c r="E151" t="s">
-        <v>382</v>
-      </c>
-      <c r="F151">
+      <c r="E151" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F151" t="s">
+        <v>382</v>
+      </c>
+      <c r="G151">
         <v>10</v>
       </c>
-      <c r="G151">
+      <c r="H151">
         <v>708</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>158</v>
       </c>
@@ -4874,17 +5330,20 @@
       <c r="D152" s="2">
         <v>22363</v>
       </c>
-      <c r="E152" t="s">
-        <v>382</v>
-      </c>
-      <c r="F152">
+      <c r="E152" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F152" t="s">
+        <v>382</v>
+      </c>
+      <c r="G152">
         <v>12</v>
       </c>
-      <c r="G152">
+      <c r="H152">
         <v>672</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>159</v>
       </c>
@@ -4897,17 +5356,20 @@
       <c r="D153" s="2">
         <v>22412</v>
       </c>
-      <c r="E153" t="s">
-        <v>382</v>
-      </c>
-      <c r="F153">
+      <c r="E153" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F153" t="s">
+        <v>382</v>
+      </c>
+      <c r="G153">
         <v>7</v>
       </c>
-      <c r="G153">
+      <c r="H153">
         <v>37</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -4920,17 +5382,20 @@
       <c r="D154" s="2">
         <v>22496</v>
       </c>
-      <c r="E154" t="s">
-        <v>382</v>
-      </c>
-      <c r="F154">
+      <c r="E154" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F154" t="s">
+        <v>382</v>
+      </c>
+      <c r="G154">
         <v>13</v>
       </c>
-      <c r="G154">
+      <c r="H154">
         <v>1020</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -4943,17 +5408,20 @@
       <c r="D155" s="2">
         <v>22594</v>
       </c>
-      <c r="E155" t="s">
-        <v>382</v>
-      </c>
-      <c r="F155">
+      <c r="E155" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F155" t="s">
+        <v>382</v>
+      </c>
+      <c r="G155">
         <v>23</v>
       </c>
-      <c r="G155">
+      <c r="H155">
         <v>340</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>162</v>
       </c>
@@ -4966,17 +5434,20 @@
       <c r="D156" s="2">
         <v>22615</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F156" t="s">
         <v>379</v>
       </c>
-      <c r="F156">
+      <c r="G156">
         <v>148</v>
       </c>
-      <c r="G156">
+      <c r="H156">
         <v>288</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>163</v>
       </c>
@@ -4989,17 +5460,20 @@
       <c r="D157" s="2">
         <v>22699</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F157" t="s">
         <v>379</v>
       </c>
-      <c r="F157">
+      <c r="G157">
         <v>139</v>
       </c>
-      <c r="G157">
+      <c r="H157">
         <v>158</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>164</v>
       </c>
@@ -5012,17 +5486,20 @@
       <c r="D158" s="2">
         <v>22741</v>
       </c>
-      <c r="E158" t="s">
-        <v>382</v>
-      </c>
-      <c r="F158">
+      <c r="E158" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F158" t="s">
+        <v>382</v>
+      </c>
+      <c r="G158">
         <v>67</v>
       </c>
-      <c r="G158">
+      <c r="H158">
         <v>559</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -5035,17 +5512,20 @@
       <c r="D159" s="2">
         <v>22748</v>
       </c>
-      <c r="E159" t="s">
-        <v>382</v>
-      </c>
-      <c r="F159">
+      <c r="E159" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F159" t="s">
+        <v>382</v>
+      </c>
+      <c r="G159">
         <v>39</v>
       </c>
-      <c r="G159">
+      <c r="H159">
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -5058,17 +5538,20 @@
       <c r="D160" s="2">
         <v>22804</v>
       </c>
-      <c r="E160" t="s">
-        <v>382</v>
-      </c>
-      <c r="F160">
+      <c r="E160" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F160" t="s">
+        <v>382</v>
+      </c>
+      <c r="G160">
         <v>10</v>
       </c>
-      <c r="G160">
+      <c r="H160">
         <v>588</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>167</v>
       </c>
@@ -5081,17 +5564,20 @@
       <c r="D161" s="2">
         <v>22811</v>
       </c>
-      <c r="E161" t="s">
-        <v>382</v>
-      </c>
-      <c r="F161">
+      <c r="E161" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F161" t="s">
+        <v>382</v>
+      </c>
+      <c r="G161">
         <v>10</v>
       </c>
-      <c r="G161">
+      <c r="H161">
         <v>912</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>168</v>
       </c>
@@ -5104,17 +5590,20 @@
       <c r="D162" s="2">
         <v>22825</v>
       </c>
-      <c r="E162" t="s">
-        <v>382</v>
-      </c>
-      <c r="F162">
+      <c r="E162" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F162" t="s">
+        <v>382</v>
+      </c>
+      <c r="G162">
         <v>16</v>
       </c>
-      <c r="G162">
+      <c r="H162">
         <v>134</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>169</v>
       </c>
@@ -5127,17 +5616,20 @@
       <c r="D163" s="2">
         <v>22832</v>
       </c>
-      <c r="E163" t="s">
-        <v>382</v>
-      </c>
-      <c r="F163">
+      <c r="E163" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F163" t="s">
+        <v>382</v>
+      </c>
+      <c r="G163">
         <v>20</v>
       </c>
-      <c r="G163">
+      <c r="H163">
         <v>212</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -5150,17 +5642,20 @@
       <c r="D164" s="2">
         <v>22860</v>
       </c>
-      <c r="E164" t="s">
-        <v>382</v>
-      </c>
-      <c r="F164">
+      <c r="E164" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F164" t="s">
+        <v>382</v>
+      </c>
+      <c r="G164">
         <v>12</v>
       </c>
-      <c r="G164">
+      <c r="H164">
         <v>268</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -5173,17 +5668,20 @@
       <c r="D165" s="2">
         <v>22867</v>
       </c>
-      <c r="E165" t="s">
-        <v>382</v>
-      </c>
-      <c r="F165">
+      <c r="E165" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F165" t="s">
+        <v>382</v>
+      </c>
+      <c r="G165">
         <v>67</v>
       </c>
-      <c r="G165">
+      <c r="H165">
         <v>131</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>172</v>
       </c>
@@ -5196,17 +5694,20 @@
       <c r="D166" s="2">
         <v>22881</v>
       </c>
-      <c r="E166" t="s">
-        <v>382</v>
-      </c>
-      <c r="F166">
+      <c r="E166" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F166" t="s">
+        <v>382</v>
+      </c>
+      <c r="G166">
         <v>67</v>
       </c>
-      <c r="G166">
+      <c r="H166">
         <v>83</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>173</v>
       </c>
@@ -5219,17 +5720,20 @@
       <c r="D167" s="2">
         <v>22951</v>
       </c>
-      <c r="E167" t="s">
-        <v>382</v>
-      </c>
-      <c r="F167">
+      <c r="E167" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F167" t="s">
+        <v>382</v>
+      </c>
+      <c r="G167">
         <v>25</v>
       </c>
-      <c r="G167">
+      <c r="H167">
         <v>52</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>174</v>
       </c>
@@ -5242,17 +5746,20 @@
       <c r="D168" s="2">
         <v>22951</v>
       </c>
-      <c r="E168" t="s">
-        <v>382</v>
-      </c>
-      <c r="F168">
+      <c r="E168" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F168" t="s">
+        <v>382</v>
+      </c>
+      <c r="G168">
         <v>55</v>
       </c>
-      <c r="G168">
+      <c r="H168">
         <v>134</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>175</v>
       </c>
@@ -5265,17 +5772,20 @@
       <c r="D169" s="2">
         <v>22958</v>
       </c>
-      <c r="E169" t="s">
-        <v>382</v>
-      </c>
-      <c r="F169">
+      <c r="E169" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F169" t="s">
+        <v>382</v>
+      </c>
+      <c r="G169">
         <v>109</v>
       </c>
-      <c r="G169">
+      <c r="H169">
         <v>580</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>176</v>
       </c>
@@ -5288,21 +5798,24 @@
       <c r="D170" s="2">
         <v>23000</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F170" t="s">
         <v>379</v>
       </c>
-      <c r="F170">
+      <c r="G170">
         <v>62</v>
       </c>
-      <c r="G170">
+      <c r="H170">
         <v>161</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>177</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="B171" s="4" t="s">
         <v>375</v>
       </c>
       <c r="C171" t="s">
@@ -5311,17 +5824,20 @@
       <c r="D171" s="2">
         <v>23007</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F171" t="s">
         <v>379</v>
       </c>
-      <c r="F171">
+      <c r="G171">
         <v>19</v>
       </c>
-      <c r="G171">
+      <c r="H171">
         <v>37</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>178</v>
       </c>
@@ -5334,17 +5850,20 @@
       <c r="D172" s="2">
         <v>23014</v>
       </c>
-      <c r="E172" t="s">
-        <v>382</v>
-      </c>
-      <c r="F172">
+      <c r="E172" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F172" t="s">
+        <v>382</v>
+      </c>
+      <c r="G172">
         <v>120</v>
       </c>
-      <c r="G172">
+      <c r="H172">
         <v>750</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>179</v>
       </c>
@@ -5357,17 +5876,20 @@
       <c r="D173" s="2">
         <v>23595</v>
       </c>
-      <c r="E173" t="s">
-        <v>382</v>
-      </c>
-      <c r="F173">
+      <c r="E173" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F173" t="s">
+        <v>382</v>
+      </c>
+      <c r="G173">
         <v>27</v>
       </c>
-      <c r="G173">
+      <c r="H173">
         <v>1164</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>180</v>
       </c>
@@ -5380,17 +5902,20 @@
       <c r="D174" s="2">
         <v>23903</v>
       </c>
-      <c r="E174" t="s">
-        <v>382</v>
-      </c>
-      <c r="F174">
+      <c r="E174" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F174" t="s">
+        <v>382</v>
+      </c>
+      <c r="G174">
         <v>8</v>
       </c>
-      <c r="G174">
+      <c r="H174">
         <v>110</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>181</v>
       </c>
@@ -5403,17 +5928,20 @@
       <c r="D175" s="2">
         <v>23903</v>
       </c>
-      <c r="E175" t="s">
-        <v>382</v>
-      </c>
-      <c r="F175">
+      <c r="E175" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F175" t="s">
+        <v>382</v>
+      </c>
+      <c r="G175">
         <v>113</v>
       </c>
-      <c r="G175">
+      <c r="H175">
         <v>840</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>184</v>
       </c>
@@ -5426,17 +5954,20 @@
       <c r="D176" s="2">
         <v>24127</v>
       </c>
-      <c r="E176" t="s">
-        <v>382</v>
-      </c>
-      <c r="F176">
+      <c r="E176" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F176" t="s">
+        <v>382</v>
+      </c>
+      <c r="G176">
         <v>28</v>
       </c>
-      <c r="G176">
+      <c r="H176">
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>182</v>
       </c>
@@ -5449,17 +5980,20 @@
       <c r="D177" s="2">
         <v>24183</v>
       </c>
-      <c r="E177" t="s">
-        <v>382</v>
-      </c>
-      <c r="F177">
+      <c r="E177" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F177" t="s">
+        <v>382</v>
+      </c>
+      <c r="G177">
         <v>13</v>
       </c>
-      <c r="G177">
+      <c r="H177">
         <v>522</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>183</v>
       </c>
@@ -5472,17 +6006,20 @@
       <c r="D178" s="2">
         <v>24211</v>
       </c>
-      <c r="E178" t="s">
-        <v>382</v>
-      </c>
-      <c r="F178">
+      <c r="E178" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F178" t="s">
+        <v>382</v>
+      </c>
+      <c r="G178">
         <v>25</v>
       </c>
-      <c r="G178">
+      <c r="H178">
         <v>500</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>185</v>
       </c>
@@ -5495,17 +6032,20 @@
       <c r="D179" s="2">
         <v>25065</v>
       </c>
-      <c r="E179" t="s">
-        <v>382</v>
-      </c>
-      <c r="F179">
+      <c r="E179" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F179" t="s">
+        <v>382</v>
+      </c>
+      <c r="G179">
         <v>114</v>
       </c>
-      <c r="G179">
+      <c r="H179">
         <v>621</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>186</v>
       </c>
@@ -5518,17 +6058,20 @@
       <c r="D180" s="2">
         <v>25128</v>
       </c>
-      <c r="E180" t="s">
-        <v>382</v>
-      </c>
-      <c r="F180">
+      <c r="E180" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F180" t="s">
+        <v>382</v>
+      </c>
+      <c r="G180">
         <v>12</v>
       </c>
-      <c r="G180">
+      <c r="H180">
         <v>416</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>187</v>
       </c>
@@ -5541,17 +6084,20 @@
       <c r="D181" s="2">
         <v>25527</v>
       </c>
-      <c r="E181" t="s">
-        <v>382</v>
-      </c>
-      <c r="F181">
+      <c r="E181" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F181" t="s">
+        <v>382</v>
+      </c>
+      <c r="G181">
         <v>100</v>
       </c>
-      <c r="G181">
+      <c r="H181">
         <v>214</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>188</v>
       </c>
@@ -5564,17 +6110,20 @@
       <c r="D182" s="2">
         <v>27788</v>
       </c>
-      <c r="E182" t="s">
-        <v>382</v>
-      </c>
-      <c r="F182">
+      <c r="E182" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F182" t="s">
+        <v>382</v>
+      </c>
+      <c r="G182">
         <v>12</v>
       </c>
-      <c r="G182">
+      <c r="H182">
         <v>628</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -5587,17 +6136,20 @@
       <c r="D183" s="2">
         <v>28474</v>
       </c>
-      <c r="E183" t="s">
-        <v>382</v>
-      </c>
-      <c r="F183">
+      <c r="E183" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F183" t="s">
+        <v>382</v>
+      </c>
+      <c r="G183">
         <v>83</v>
       </c>
-      <c r="G183">
+      <c r="H183">
         <v>494</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>190</v>
       </c>
@@ -5610,17 +6162,20 @@
       <c r="D184" s="2">
         <v>19480</v>
       </c>
-      <c r="E184" t="s">
-        <v>382</v>
-      </c>
-      <c r="F184">
+      <c r="E184" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F184" t="s">
+        <v>382</v>
+      </c>
+      <c r="G184">
         <v>25</v>
       </c>
-      <c r="G184">
+      <c r="H184">
         <v>81</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>191</v>
       </c>
@@ -5633,17 +6188,20 @@
       <c r="D185" s="2">
         <v>19968</v>
       </c>
-      <c r="E185" t="s">
-        <v>382</v>
-      </c>
-      <c r="F185">
+      <c r="E185" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F185" t="s">
+        <v>382</v>
+      </c>
+      <c r="G185">
         <v>18</v>
       </c>
-      <c r="G185">
+      <c r="H185">
         <v>144</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>192</v>
       </c>
@@ -5656,17 +6214,20 @@
       <c r="D186" s="2">
         <v>21186</v>
       </c>
-      <c r="E186" t="s">
-        <v>382</v>
-      </c>
-      <c r="F186">
+      <c r="E186" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F186" t="s">
+        <v>382</v>
+      </c>
+      <c r="G186">
         <v>10</v>
       </c>
-      <c r="G186">
+      <c r="H186">
         <v>438</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>193</v>
       </c>
@@ -5679,17 +6240,20 @@
       <c r="D187" s="2">
         <v>22555</v>
       </c>
-      <c r="E187" t="s">
-        <v>382</v>
-      </c>
-      <c r="F187">
+      <c r="E187" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F187" t="s">
+        <v>382</v>
+      </c>
+      <c r="G187">
         <v>9</v>
       </c>
-      <c r="G187">
+      <c r="H187">
         <v>110</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>194</v>
       </c>
@@ -5702,17 +6266,20 @@
       <c r="D188" s="2">
         <v>24228</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F188" t="s">
         <v>379</v>
       </c>
-      <c r="F188">
+      <c r="G188">
         <v>13</v>
       </c>
-      <c r="G188">
+      <c r="H188">
         <v>346</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>195</v>
       </c>
@@ -5725,13 +6292,16 @@
       <c r="D189" s="2">
         <v>24198</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E189" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F189" t="s">
         <v>379</v>
       </c>
-      <c r="F189">
+      <c r="G189">
         <v>13</v>
       </c>
-      <c r="G189">
+      <c r="H189">
         <v>496</v>
       </c>
     </row>

</xml_diff>